<commit_message>
:zap: general update, add substring search time graph
</commit_message>
<xml_diff>
--- a/docs/Practical 7 - Search Time Graph.xlsx
+++ b/docs/Practical 7 - Search Time Graph.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajit Banerjee\Desktop\Algorithms\algorithm-portfolio-20290-rajitbanerjee\src\p7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajit Banerjee\Desktop\Algorithms\algorithm-portfolio-20290-rajitbanerjee\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377574AA-E4CC-4EA1-99D4-6645534E4B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826871E3-1A98-439B-A31D-192D31150561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>TEXT SIZE</t>
+    <t>Text Size</t>
   </si>
   <si>
-    <t>BRUTE FORCE SEARCH</t>
+    <t>Brute Force Search</t>
   </si>
   <si>
-    <t>KMP SEARCH</t>
+    <t>KMP Search</t>
+  </si>
+  <si>
+    <t>Index (BF)</t>
+  </si>
+  <si>
+    <t>Index (KMP)</t>
+  </si>
+  <si>
+    <t>Knuth-Morris-Pratt algorithm is clearly faster than a brute force search.</t>
+  </si>
+  <si>
+    <t>In general, KMP search has complexity O(m + n), whereas a brute force search is O(m*n),</t>
+  </si>
+  <si>
+    <t>where m is pattern length, n is text length.</t>
   </si>
 </sst>
 </file>
@@ -69,10 +84,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -180,7 +198,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BRUTE FORCE SEARCH</c:v>
+                  <c:v>Brute Force Search</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -211,120 +229,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>426</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>524</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>587</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>810500</c:v>
+                  <c:v>9900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2300</c:v>
+                  <c:v>14700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2800</c:v>
+                  <c:v>37600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4500</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>19400</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>40700</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>78400</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>49400</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>133000</c:v>
+                  <c:v>79900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,7 +272,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-39F5-42DA-80D0-3FCDA97CA12E}"/>
+              <c16:uniqueId val="{00000000-27B6-48D3-9047-CD7D40A4D23F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -345,7 +285,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KMP SEARCH</c:v>
+                  <c:v>KMP Search</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -376,120 +316,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>426</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>524</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>587</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$18</c:f>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>457600</c:v>
+                  <c:v>8500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2100</c:v>
+                  <c:v>10900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>29000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4100</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>33500</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>55700</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30100</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>67300</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>83300</c:v>
+                  <c:v>44500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,7 +359,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-39F5-42DA-80D0-3FCDA97CA12E}"/>
+              <c16:uniqueId val="{00000001-27B6-48D3-9047-CD7D40A4D23F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -638,6 +500,7 @@
         <c:axId val="328419167"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1394,16 +1257,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1694,21 +1557,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1718,203 +1583,111 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>810500</v>
+        <v>1594500</v>
       </c>
       <c r="C2" s="1">
-        <v>457600</v>
+        <v>1004600</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9900</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8500</v>
+      </c>
+      <c r="D3" s="1">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1">
+        <v>14700</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10900</v>
+      </c>
+      <c r="D4" s="1">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>147</v>
+      </c>
+      <c r="B5" s="1">
+        <v>37600</v>
+      </c>
+      <c r="C5" s="1">
+        <v>29000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>142</v>
+      </c>
+      <c r="E5" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>154</v>
+      </c>
+      <c r="B6" s="1">
+        <v>79900</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44500</v>
+      </c>
+      <c r="D6" s="1">
+        <v>149</v>
+      </c>
+      <c r="E6" s="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <v>2300</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2100</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2800</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3000</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>27</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2000</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>38</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2500</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>63</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4600</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>77</v>
-      </c>
-      <c r="B9" s="1">
-        <v>4600</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>88</v>
-      </c>
-      <c r="B10" s="1">
-        <v>6000</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>98</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2200</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>113</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7100</v>
-      </c>
-      <c r="C12" s="1">
-        <v>6100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>165</v>
-      </c>
-      <c r="B13" s="1">
-        <v>4500</v>
-      </c>
-      <c r="C13" s="1">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>252</v>
-      </c>
-      <c r="B14" s="1">
-        <v>19400</v>
-      </c>
-      <c r="C14" s="1">
-        <v>33500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>316</v>
-      </c>
-      <c r="B15" s="1">
-        <v>40700</v>
-      </c>
-      <c r="C15" s="1">
-        <v>55700</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>426</v>
-      </c>
-      <c r="B16" s="1">
-        <v>78400</v>
-      </c>
-      <c r="C16" s="1">
-        <v>30100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>524</v>
-      </c>
-      <c r="B17" s="1">
-        <v>49400</v>
-      </c>
-      <c r="C17" s="1">
-        <v>67300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>587</v>
-      </c>
-      <c r="B18" s="1">
-        <v>133000</v>
-      </c>
-      <c r="C18" s="1">
-        <v>83300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>5549</v>
-      </c>
-      <c r="B19" s="1">
-        <v>295700</v>
-      </c>
-      <c r="C19" s="1">
-        <v>194900</v>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>